<commit_message>
binary and multiclass fitting and fishing effort checks
</commit_message>
<xml_diff>
--- a/results/modelFittingComparison.xlsx
+++ b/results/modelFittingComparison.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jsala\ownCloud\papers\paperPeixBlau\PS_ML_git\PurseSeine_RandomForest\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E49DB4E-55B0-4A2B-B7E9-C7630606BA54}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{706FBB3A-6D72-4D5D-B980-BC7EB2006931}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="52">
   <si>
     <t>bootstrap</t>
   </si>
@@ -160,13 +160,34 @@
   </si>
   <si>
     <t>manually set to avoid overfitting</t>
+  </si>
+  <si>
+    <t>model fitting process</t>
+  </si>
+  <si>
+    <t>1. Bootstrap = True. Otherwise can not set max_samples</t>
+  </si>
+  <si>
+    <t>2. Check max_depth effect on overfitting. Set max_depth</t>
+  </si>
+  <si>
+    <t>3. General fitting for other parameters: max_features, max_leaf_nodes, max_samples, min_impurity_decrease, min_samples_leaf, min_samples_split</t>
+  </si>
+  <si>
+    <t>4. Min_impurity_decrease clearly affect performance. Set to 0</t>
+  </si>
+  <si>
+    <t>5. GridSearchCV with other parameters</t>
+  </si>
+  <si>
+    <t>0.Splitting with general good results</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -182,6 +203,12 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Consolas"/>
@@ -237,7 +264,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -264,6 +291,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -544,10 +572,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M40"/>
+  <dimension ref="A1:M49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1087,6 +1115,9 @@
       <c r="A22" s="4" t="s">
         <v>33</v>
       </c>
+      <c r="D22" s="12" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
@@ -1095,6 +1126,9 @@
       <c r="B23" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="D23" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
@@ -1106,6 +1140,12 @@
       <c r="C24" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="D24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
@@ -1117,6 +1157,12 @@
       <c r="C25" s="2">
         <v>10</v>
       </c>
+      <c r="D25" s="2">
+        <v>6</v>
+      </c>
+      <c r="E25">
+        <v>6</v>
+      </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
@@ -1128,6 +1174,12 @@
       <c r="C26" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="D26" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
@@ -1139,6 +1191,12 @@
       <c r="C27" s="2">
         <v>1000</v>
       </c>
+      <c r="D27" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E27">
+        <v>1000</v>
+      </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
@@ -1150,6 +1208,12 @@
       <c r="C28" s="2" t="s">
         <v>35</v>
       </c>
+      <c r="D28" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
@@ -1161,6 +1225,12 @@
       <c r="C29" s="2">
         <v>0</v>
       </c>
+      <c r="D29" s="2">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
@@ -1172,6 +1242,12 @@
       <c r="C30" s="2">
         <v>1</v>
       </c>
+      <c r="D30" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E30" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
@@ -1183,6 +1259,12 @@
       <c r="C31" s="2">
         <v>4</v>
       </c>
+      <c r="D31" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E31">
+        <v>3</v>
+      </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
@@ -1194,8 +1276,14 @@
       <c r="C32" s="2">
         <v>100</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D32" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E32" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>31</v>
       </c>
@@ -1203,7 +1291,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>30</v>
       </c>
@@ -1211,46 +1299,99 @@
         <v>384000</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>23</v>
       </c>
       <c r="C35" s="2">
         <v>0.93</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E35">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>24</v>
       </c>
       <c r="C36" s="2">
         <v>0.83</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E36">
+        <v>0.79</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>10</v>
       </c>
       <c r="C37" s="2">
         <v>0.81</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E37">
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>11</v>
       </c>
       <c r="C38" s="2">
         <v>0.84</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E38">
+        <v>0.73</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E39">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>39</v>
+      </c>
+      <c r="E40">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" s="12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" s="14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" s="14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" s="14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" s="14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" s="14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49" s="14" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>